<commit_message>
Added new action for Shopping cart website
</commit_message>
<xml_diff>
--- a/MBT_UFTOne_Samples/Default.xlsx
+++ b/MBT_UFTOne_Samples/Default.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="SpreadsheetGear 8.2.5.102"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="RegisterNewUser" sheetId="3" r:id="rId3"/>
     <sheet name="OpenNewAccount" sheetId="4" r:id="rId4"/>
     <sheet name="Logout" sheetId="5" r:id="rId5"/>
+    <sheet name="UserLogin_Shopping" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="40001"/>
 </workbook>
@@ -495,12 +496,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.95"/>
+  <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
     <col min="1" max="16384" width="8.8984375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1"/>
+    <row r="1" ht="14.95" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -548,7 +549,7 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -561,4 +562,23 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.1"/>
+  <cols>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>